<commit_message>
Add parsing multiple files to excel and start with some data validation
</commit_message>
<xml_diff>
--- a/src/splitwise_invoicing/TemplateExcel.xlsx
+++ b/src/splitwise_invoicing/TemplateExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calga\Documents\gitHubRepos\splitwise-invoicing\src\splitwise_invoicing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D9BC5C-F8CB-4B89-B482-CE08052F9B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B490712-F2AE-421E-9877-47FBD320ACAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11835" xr2:uid="{A22465D9-0DBF-4442-A5D7-709D28AD057B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A22465D9-0DBF-4442-A5D7-709D28AD057B}"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Received Date</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Add to Splitwise? (TRUE/FALSE)</t>
+  </si>
+  <si>
+    <t>Splitwise Group</t>
+  </si>
+  <si>
+    <t>Add To Splitwise Options</t>
   </si>
 </sst>
 </file>
@@ -126,7 +132,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF33CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -464,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA687DB4-DCEE-430B-9641-EAB787303D4C}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,12 +504,13 @@
     <col min="3" max="3" width="58.140625" customWidth="1"/>
     <col min="4" max="4" width="8.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="30" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,17 +527,20 @@
         <v>9</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:G1048576">
+  <conditionalFormatting sqref="E2:E1048576 G2:H1048576">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND(E2=FALSE, ISBLANK(E2)=FALSE)</formula>
     </cfRule>
@@ -522,30 +553,54 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{7FD3DD71-1A25-447B-BAC1-60055F16F350}">
+          <x14:formula1>
+            <xm:f>Config!$B$2:$B$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D948B0D3-0B1B-4C16-A02A-6272023E65BA}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish a validation on columns
</commit_message>
<xml_diff>
--- a/src/splitwise_invoicing/TemplateExcel.xlsx
+++ b/src/splitwise_invoicing/TemplateExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calga\Documents\gitHubRepos\splitwise-invoicing\src\splitwise_invoicing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B490712-F2AE-421E-9877-47FBD320ACAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606C919C-C6AF-47F0-9F8F-AB68BCE37D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A22465D9-0DBF-4442-A5D7-709D28AD057B}"/>
   </bookViews>
@@ -132,28 +132,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF33CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -493,9 +472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA687DB4-DCEE-430B-9641-EAB787303D4C}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -553,18 +530,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{7FD3DD71-1A25-447B-BAC1-60055F16F350}">
-          <x14:formula1>
-            <xm:f>Config!$B$2:$B$1048576</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -572,9 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D948B0D3-0B1B-4C16-A02A-6272023E65BA}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Add currency column and function to write
</commit_message>
<xml_diff>
--- a/src/splitwise_invoicing/TemplateExcel.xlsx
+++ b/src/splitwise_invoicing/TemplateExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calga\Documents\GitHubRepos\splitwise-invoicing\src\splitwise_invoicing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E21CC53-B45F-4BBD-B06A-4A1D90933493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23020048-7641-4867-B906-C70C03854B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6975" yWindow="9825" windowWidth="28800" windowHeight="15435" xr2:uid="{A22465D9-0DBF-4442-A5D7-709D28AD057B}"/>
+    <workbookView xWindow="5085" yWindow="3120" windowWidth="28800" windowHeight="15435" xr2:uid="{A22465D9-0DBF-4442-A5D7-709D28AD057B}"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Transaction Date</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Card</t>
+  </si>
+  <si>
+    <t>Currency</t>
   </si>
 </sst>
 </file>
@@ -470,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA687DB4-DCEE-430B-9641-EAB787303D4C}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,14 +485,15 @@
     <col min="2" max="2" width="22.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="58.140625" customWidth="1"/>
     <col min="4" max="4" width="8.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="30" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -502,32 +506,35 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E1048576 G2:H1048576">
+  <conditionalFormatting sqref="F2:F1048576 H2:I1048576">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>AND(E2=FALSE, ISBLANK(E2)=FALSE)</formula>
+      <formula>AND(F2=FALSE, ISBLANK(F2)=FALSE)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>E2=TRUE</formula>
+      <formula>F2=TRUE</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>AND(E2&lt;&gt;TRUE, E2&lt;&gt;FALSE)</formula>
+      <formula>AND(F2&lt;&gt;TRUE, F2&lt;&gt;FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -539,7 +546,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D948B0D3-0B1B-4C16-A02A-6272023E65BA}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B2:B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>